<commit_message>
Minor changes, everything should be working properly
</commit_message>
<xml_diff>
--- a/AnimalCounts.xlsx
+++ b/AnimalCounts.xlsx
@@ -12,12 +12,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Turn</t>
   </si>
   <si>
+    <t>Bear</t>
+  </si>
+  <si>
     <t>Hare</t>
+  </si>
+  <si>
+    <t>Deer</t>
   </si>
   <si>
     <t>Fox</t>
@@ -93,16 +99,16 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Hare</c:v>
+            <c:v>Bear</c:v>
           </c:tx>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>AnimalCounts!$A$2:$A$82</c:f>
+              <c:f>AnimalCounts!$A$2:$A$72</c:f>
               <c:numCache>
-                <c:ptCount val="81"/>
+                <c:ptCount val="71"/>
                 <c:pt idx="0">
                   <c:v>0.0</c:v>
                 </c:pt>
@@ -315,287 +321,227 @@
                 </c:pt>
                 <c:pt idx="70">
                   <c:v>70.0</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>71.0</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>72.0</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>73.0</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>74.0</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>75.0</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>76.0</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>77.0</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>78.0</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>79.0</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>80.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>AnimalCounts!$B$2:$B$82</c:f>
+              <c:f>AnimalCounts!$B$2:$B$72</c:f>
               <c:numCache>
-                <c:ptCount val="81"/>
+                <c:ptCount val="71"/>
                 <c:pt idx="0">
                   <c:v>50.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.0</c:v>
+                  <c:v>50.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.0</c:v>
+                  <c:v>50.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.0</c:v>
+                  <c:v>51.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.0</c:v>
+                  <c:v>51.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10.0</c:v>
+                  <c:v>51.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>12.0</c:v>
+                  <c:v>51.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>14.0</c:v>
+                  <c:v>51.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>15.0</c:v>
+                  <c:v>51.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>17.0</c:v>
+                  <c:v>51.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>19.0</c:v>
+                  <c:v>51.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>21.0</c:v>
+                  <c:v>51.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>23.0</c:v>
+                  <c:v>51.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>25.0</c:v>
+                  <c:v>51.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>27.0</c:v>
+                  <c:v>52.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>29.0</c:v>
+                  <c:v>52.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>31.0</c:v>
+                  <c:v>52.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>33.0</c:v>
+                  <c:v>53.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>35.0</c:v>
+                  <c:v>53.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>36.0</c:v>
+                  <c:v>53.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>38.0</c:v>
+                  <c:v>53.0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>40.0</c:v>
+                  <c:v>53.0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>40.0</c:v>
+                  <c:v>53.0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>40.0</c:v>
+                  <c:v>53.0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>41.0</c:v>
+                  <c:v>53.0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>41.0</c:v>
+                  <c:v>53.0</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>40.0</c:v>
+                  <c:v>53.0</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>40.0</c:v>
+                  <c:v>53.0</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>40.0</c:v>
+                  <c:v>53.0</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>40.0</c:v>
+                  <c:v>55.0</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>40.0</c:v>
+                  <c:v>56.0</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>39.0</c:v>
+                  <c:v>56.0</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>39.0</c:v>
+                  <c:v>56.0</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>38.0</c:v>
+                  <c:v>56.0</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>38.0</c:v>
+                  <c:v>56.0</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>38.0</c:v>
+                  <c:v>56.0</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>38.0</c:v>
+                  <c:v>56.0</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>38.0</c:v>
+                  <c:v>56.0</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>38.0</c:v>
+                  <c:v>56.0</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>39.0</c:v>
+                  <c:v>56.0</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>39.0</c:v>
+                  <c:v>56.0</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>39.0</c:v>
+                  <c:v>56.0</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>39.0</c:v>
+                  <c:v>56.0</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>40.0</c:v>
+                  <c:v>56.0</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>40.0</c:v>
+                  <c:v>57.0</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>40.0</c:v>
+                  <c:v>58.0</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>39.0</c:v>
+                  <c:v>58.0</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>38.0</c:v>
+                  <c:v>59.0</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>38.0</c:v>
+                  <c:v>59.0</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>36.0</c:v>
+                  <c:v>59.0</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>36.0</c:v>
+                  <c:v>59.0</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>37.0</c:v>
+                  <c:v>59.0</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>37.0</c:v>
+                  <c:v>60.0</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>36.0</c:v>
+                  <c:v>61.0</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>36.0</c:v>
+                  <c:v>61.0</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>37.0</c:v>
+                  <c:v>61.0</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>37.0</c:v>
+                  <c:v>61.0</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>37.0</c:v>
+                  <c:v>61.0</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>37.0</c:v>
+                  <c:v>61.0</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>38.0</c:v>
+                  <c:v>61.0</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>37.0</c:v>
+                  <c:v>61.0</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>36.0</c:v>
+                  <c:v>61.0</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>36.0</c:v>
+                  <c:v>62.0</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>37.0</c:v>
+                  <c:v>62.0</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>36.0</c:v>
+                  <c:v>62.0</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>36.0</c:v>
+                  <c:v>62.0</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>36.0</c:v>
+                  <c:v>63.0</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>36.0</c:v>
+                  <c:v>63.0</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>36.0</c:v>
+                  <c:v>63.0</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>37.0</c:v>
+                  <c:v>63.0</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>37.0</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>37.0</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>38.0</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>37.0</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>37.0</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>37.0</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>38.0</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>40.0</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>40.0</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>40.0</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>41.0</c:v>
+                  <c:v>63.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -605,6 +551,910 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
+            <c:v>Hare</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>AnimalCounts!$A$2:$A$72</c:f>
+              <c:numCache>
+                <c:ptCount val="71"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>17.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>18.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>19.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>21.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>22.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>24.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>26.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>27.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>28.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>29.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>31.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>33.0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>34.0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>35.0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>36.0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>37.0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>38.0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>39.0</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>41.0</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>43.0</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>44.0</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>45.0</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>46.0</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>48.0</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>49.0</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>51.0</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>52.0</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>53.0</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>54.0</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>55.0</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>56.0</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>57.0</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>58.0</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>59.0</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>60.0</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>61.0</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>62.0</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>63.0</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>64.0</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>65.0</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>66.0</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>67.0</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>68.0</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>69.0</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>70.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>AnimalCounts!$C$2:$C$72</c:f>
+              <c:numCache>
+                <c:ptCount val="71"/>
+                <c:pt idx="0">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>49.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>49.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>46.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>45.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>48.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>43.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>48.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>48.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>46.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>46.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>45.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>46.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>44.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>44.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>43.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>38.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>38.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>38.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>38.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>37.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>37.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>49.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>44.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>37.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>44.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>37.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>36.0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>34.0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>48.0</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>45.0</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>49.0</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>49.0</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>49.0</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>49.0</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>45.0</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>45.0</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>45.0</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>45.0</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>45.0</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>44.0</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>43.0</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>43.0</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>43.0</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>41.0</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>41.0</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>41.0</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>41.0</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>41.0</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>41.0</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>41.0</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>39.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Deer</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>AnimalCounts!$A$2:$A$72</c:f>
+              <c:numCache>
+                <c:ptCount val="71"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>17.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>18.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>19.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>21.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>22.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>24.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>26.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>27.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>28.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>29.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>31.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>33.0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>34.0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>35.0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>36.0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>37.0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>38.0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>39.0</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>41.0</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>43.0</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>44.0</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>45.0</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>46.0</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>48.0</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>49.0</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>51.0</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>52.0</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>53.0</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>54.0</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>55.0</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>56.0</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>57.0</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>58.0</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>59.0</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>60.0</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>61.0</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>62.0</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>63.0</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>64.0</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>65.0</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>66.0</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>67.0</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>68.0</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>69.0</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>70.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>AnimalCounts!$D$2:$D$72</c:f>
+              <c:numCache>
+                <c:ptCount val="71"/>
+                <c:pt idx="0">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>49.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>49.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>48.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>49.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>49.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>48.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>48.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>48.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>49.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>49.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>41.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>41.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>39.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>39.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>38.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>48.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>48.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>48.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>49.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>44.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>44.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>37.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>44.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>37.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>48.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>49.0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>49.0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>49.0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>49.0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>49.0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>49.0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>48.0</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>45.0</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>45.0</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>45.0</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>45.0</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>48.0</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>45.0</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>46.0</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>46.0</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>45.0</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>46.0</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>41.0</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>41.0</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>46.0</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>46.0</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>45.0</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>48.0</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>49.0</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>49.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
             <c:v>Fox</c:v>
           </c:tx>
           <c:marker>
@@ -612,9 +1462,9 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>AnimalCounts!$A$2:$A$82</c:f>
+              <c:f>AnimalCounts!$A$2:$A$72</c:f>
               <c:numCache>
-                <c:ptCount val="81"/>
+                <c:ptCount val="71"/>
                 <c:pt idx="0">
                   <c:v>0.0</c:v>
                 </c:pt>
@@ -827,65 +1677,35 @@
                 </c:pt>
                 <c:pt idx="70">
                   <c:v>70.0</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>71.0</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>72.0</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>73.0</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>74.0</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>75.0</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>76.0</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>77.0</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>78.0</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>79.0</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>80.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>AnimalCounts!$C$2:$C$82</c:f>
+              <c:f>AnimalCounts!$E$2:$E$72</c:f>
               <c:numCache>
-                <c:ptCount val="81"/>
+                <c:ptCount val="71"/>
                 <c:pt idx="0">
                   <c:v>50.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>50.0</c:v>
+                  <c:v>49.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>50.0</c:v>
+                  <c:v>49.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>50.0</c:v>
+                  <c:v>49.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>50.0</c:v>
+                  <c:v>49.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>50.0</c:v>
+                  <c:v>48.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>50.0</c:v>
+                  <c:v>44.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>50.0</c:v>
@@ -894,220 +1714,190 @@
                   <c:v>50.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>50.0</c:v>
+                  <c:v>48.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>50.0</c:v>
+                  <c:v>42.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>50.0</c:v>
+                  <c:v>42.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>50.0</c:v>
+                  <c:v>42.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>50.0</c:v>
+                  <c:v>48.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>50.0</c:v>
+                  <c:v>48.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>50.0</c:v>
+                  <c:v>48.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>50.0</c:v>
+                  <c:v>48.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>50.0</c:v>
+                  <c:v>48.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>50.0</c:v>
+                  <c:v>49.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>50.0</c:v>
+                  <c:v>47.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>50.0</c:v>
+                  <c:v>46.0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>50.0</c:v>
+                  <c:v>47.0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>50.0</c:v>
+                  <c:v>41.0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>50.0</c:v>
+                  <c:v>42.0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>50.0</c:v>
+                  <c:v>42.0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>50.0</c:v>
+                  <c:v>42.0</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>50.0</c:v>
+                  <c:v>43.0</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>50.0</c:v>
+                  <c:v>37.0</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>50.0</c:v>
+                  <c:v>37.0</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>50.0</c:v>
+                  <c:v>48.0</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>50.0</c:v>
+                  <c:v>48.0</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>50.0</c:v>
+                  <c:v>48.0</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>50.0</c:v>
+                  <c:v>45.0</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>50.0</c:v>
+                  <c:v>45.0</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>50.0</c:v>
+                  <c:v>44.0</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>50.0</c:v>
+                  <c:v>43.0</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>50.0</c:v>
+                  <c:v>43.0</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>50.0</c:v>
+                  <c:v>44.0</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>50.0</c:v>
+                  <c:v>45.0</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>50.0</c:v>
+                  <c:v>45.0</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>50.0</c:v>
+                  <c:v>30.0</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>50.0</c:v>
+                  <c:v>29.0</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>50.0</c:v>
+                  <c:v>29.0</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>50.0</c:v>
+                  <c:v>29.0</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>50.0</c:v>
+                  <c:v>29.0</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>50.0</c:v>
+                  <c:v>29.0</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>50.0</c:v>
+                  <c:v>29.0</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>50.0</c:v>
+                  <c:v>29.0</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>50.0</c:v>
+                  <c:v>29.0</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>50.0</c:v>
+                  <c:v>29.0</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>50.0</c:v>
+                  <c:v>28.0</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>50.0</c:v>
+                  <c:v>28.0</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>50.0</c:v>
+                  <c:v>28.0</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>50.0</c:v>
+                  <c:v>26.0</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>50.0</c:v>
+                  <c:v>26.0</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>50.0</c:v>
+                  <c:v>26.0</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>50.0</c:v>
+                  <c:v>25.0</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>50.0</c:v>
+                  <c:v>25.0</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>50.0</c:v>
+                  <c:v>25.0</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>50.0</c:v>
+                  <c:v>25.0</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>50.0</c:v>
+                  <c:v>25.0</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>50.0</c:v>
+                  <c:v>25.0</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>50.0</c:v>
+                  <c:v>25.0</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>50.0</c:v>
+                  <c:v>25.0</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>50.0</c:v>
+                  <c:v>25.0</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>50.0</c:v>
+                  <c:v>25.0</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>50.0</c:v>
+                  <c:v>25.0</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>50.0</c:v>
+                  <c:v>24.0</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>50.0</c:v>
+                  <c:v>23.0</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>50.0</c:v>
+                  <c:v>23.0</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>50.0</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>50.0</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>50.0</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>50.0</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>50.0</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>50.0</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>50.0</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>50.0</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>50.0</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>50.0</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>50.0</c:v>
+                  <c:v>23.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1206,13 +1996,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>83</xdr:row>
+      <xdr:row>73</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>101</xdr:row>
+      <xdr:row>91</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
@@ -1237,7 +2027,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D82"/>
+  <dimension ref="A1:E72"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -1253,6 +2043,12 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -1264,19 +2060,28 @@
       <c r="C2" t="n">
         <v>50.0</v>
       </c>
+      <c r="D2" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>50.0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
         <v>1.0</v>
       </c>
       <c r="B3" t="n">
-        <v>2.0</v>
+        <v>50.0</v>
       </c>
       <c r="C3" t="n">
-        <v>50.0</v>
+        <v>49.0</v>
       </c>
       <c r="D3" t="n">
-        <v>50.0</v>
+        <v>49.0</v>
+      </c>
+      <c r="E3" t="n">
+        <v>49.0</v>
       </c>
     </row>
     <row r="4">
@@ -1284,13 +2089,16 @@
         <v>2.0</v>
       </c>
       <c r="B4" t="n">
-        <v>4.0</v>
+        <v>50.0</v>
       </c>
       <c r="C4" t="n">
-        <v>50.0</v>
+        <v>49.0</v>
       </c>
       <c r="D4" t="n">
-        <v>50.0</v>
+        <v>47.0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>49.0</v>
       </c>
     </row>
     <row r="5">
@@ -1298,13 +2106,16 @@
         <v>3.0</v>
       </c>
       <c r="B5" t="n">
-        <v>6.0</v>
+        <v>51.0</v>
       </c>
       <c r="C5" t="n">
-        <v>50.0</v>
+        <v>47.0</v>
       </c>
       <c r="D5" t="n">
-        <v>50.0</v>
+        <v>49.0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>49.0</v>
       </c>
     </row>
     <row r="6">
@@ -1312,13 +2123,16 @@
         <v>4.0</v>
       </c>
       <c r="B6" t="n">
-        <v>8.0</v>
+        <v>51.0</v>
       </c>
       <c r="C6" t="n">
-        <v>50.0</v>
+        <v>46.0</v>
       </c>
       <c r="D6" t="n">
-        <v>50.0</v>
+        <v>48.0</v>
+      </c>
+      <c r="E6" t="n">
+        <v>49.0</v>
       </c>
     </row>
     <row r="7">
@@ -1326,13 +2140,16 @@
         <v>5.0</v>
       </c>
       <c r="B7" t="n">
-        <v>10.0</v>
+        <v>51.0</v>
       </c>
       <c r="C7" t="n">
-        <v>50.0</v>
+        <v>45.0</v>
       </c>
       <c r="D7" t="n">
-        <v>50.0</v>
+        <v>49.0</v>
+      </c>
+      <c r="E7" t="n">
+        <v>48.0</v>
       </c>
     </row>
     <row r="8">
@@ -1340,13 +2157,16 @@
         <v>6.0</v>
       </c>
       <c r="B8" t="n">
-        <v>12.0</v>
+        <v>51.0</v>
       </c>
       <c r="C8" t="n">
-        <v>50.0</v>
+        <v>48.0</v>
       </c>
       <c r="D8" t="n">
-        <v>50.0</v>
+        <v>49.0</v>
+      </c>
+      <c r="E8" t="n">
+        <v>44.0</v>
       </c>
     </row>
     <row r="9">
@@ -1354,12 +2174,15 @@
         <v>7.0</v>
       </c>
       <c r="B9" t="n">
-        <v>14.0</v>
+        <v>51.0</v>
       </c>
       <c r="C9" t="n">
-        <v>50.0</v>
+        <v>43.0</v>
       </c>
       <c r="D9" t="n">
+        <v>48.0</v>
+      </c>
+      <c r="E9" t="n">
         <v>50.0</v>
       </c>
     </row>
@@ -1368,12 +2191,15 @@
         <v>8.0</v>
       </c>
       <c r="B10" t="n">
-        <v>15.0</v>
+        <v>51.0</v>
       </c>
       <c r="C10" t="n">
-        <v>50.0</v>
+        <v>42.0</v>
       </c>
       <c r="D10" t="n">
+        <v>48.0</v>
+      </c>
+      <c r="E10" t="n">
         <v>50.0</v>
       </c>
     </row>
@@ -1382,13 +2208,16 @@
         <v>9.0</v>
       </c>
       <c r="B11" t="n">
-        <v>17.0</v>
+        <v>51.0</v>
       </c>
       <c r="C11" t="n">
-        <v>50.0</v>
+        <v>42.0</v>
       </c>
       <c r="D11" t="n">
         <v>50.0</v>
+      </c>
+      <c r="E11" t="n">
+        <v>48.0</v>
       </c>
     </row>
     <row r="12">
@@ -1396,13 +2225,16 @@
         <v>10.0</v>
       </c>
       <c r="B12" t="n">
-        <v>19.0</v>
+        <v>51.0</v>
       </c>
       <c r="C12" t="n">
         <v>50.0</v>
       </c>
       <c r="D12" t="n">
-        <v>50.0</v>
+        <v>48.0</v>
+      </c>
+      <c r="E12" t="n">
+        <v>42.0</v>
       </c>
     </row>
     <row r="13">
@@ -1410,13 +2242,16 @@
         <v>11.0</v>
       </c>
       <c r="B13" t="n">
-        <v>21.0</v>
+        <v>51.0</v>
       </c>
       <c r="C13" t="n">
-        <v>50.0</v>
+        <v>48.0</v>
       </c>
       <c r="D13" t="n">
-        <v>50.0</v>
+        <v>49.0</v>
+      </c>
+      <c r="E13" t="n">
+        <v>42.0</v>
       </c>
     </row>
     <row r="14">
@@ -1424,13 +2259,16 @@
         <v>12.0</v>
       </c>
       <c r="B14" t="n">
-        <v>23.0</v>
+        <v>51.0</v>
       </c>
       <c r="C14" t="n">
-        <v>50.0</v>
+        <v>48.0</v>
       </c>
       <c r="D14" t="n">
-        <v>50.0</v>
+        <v>49.0</v>
+      </c>
+      <c r="E14" t="n">
+        <v>42.0</v>
       </c>
     </row>
     <row r="15">
@@ -1438,13 +2276,16 @@
         <v>13.0</v>
       </c>
       <c r="B15" t="n">
-        <v>25.0</v>
+        <v>51.0</v>
       </c>
       <c r="C15" t="n">
-        <v>50.0</v>
+        <v>47.0</v>
       </c>
       <c r="D15" t="n">
-        <v>50.0</v>
+        <v>41.0</v>
+      </c>
+      <c r="E15" t="n">
+        <v>48.0</v>
       </c>
     </row>
     <row r="16">
@@ -1452,13 +2293,16 @@
         <v>14.0</v>
       </c>
       <c r="B16" t="n">
-        <v>27.0</v>
+        <v>52.0</v>
       </c>
       <c r="C16" t="n">
-        <v>50.0</v>
+        <v>46.0</v>
       </c>
       <c r="D16" t="n">
-        <v>50.0</v>
+        <v>41.0</v>
+      </c>
+      <c r="E16" t="n">
+        <v>48.0</v>
       </c>
     </row>
     <row r="17">
@@ -1466,13 +2310,16 @@
         <v>15.0</v>
       </c>
       <c r="B17" t="n">
-        <v>29.0</v>
+        <v>52.0</v>
       </c>
       <c r="C17" t="n">
-        <v>50.0</v>
+        <v>46.0</v>
       </c>
       <c r="D17" t="n">
-        <v>50.0</v>
+        <v>40.0</v>
+      </c>
+      <c r="E17" t="n">
+        <v>48.0</v>
       </c>
     </row>
     <row r="18">
@@ -1480,13 +2327,16 @@
         <v>16.0</v>
       </c>
       <c r="B18" t="n">
-        <v>31.0</v>
+        <v>52.0</v>
       </c>
       <c r="C18" t="n">
-        <v>50.0</v>
+        <v>45.0</v>
       </c>
       <c r="D18" t="n">
-        <v>50.0</v>
+        <v>40.0</v>
+      </c>
+      <c r="E18" t="n">
+        <v>48.0</v>
       </c>
     </row>
     <row r="19">
@@ -1494,13 +2344,16 @@
         <v>17.0</v>
       </c>
       <c r="B19" t="n">
-        <v>33.0</v>
+        <v>53.0</v>
       </c>
       <c r="C19" t="n">
-        <v>50.0</v>
+        <v>46.0</v>
       </c>
       <c r="D19" t="n">
-        <v>50.0</v>
+        <v>40.0</v>
+      </c>
+      <c r="E19" t="n">
+        <v>48.0</v>
       </c>
     </row>
     <row r="20">
@@ -1508,13 +2361,16 @@
         <v>18.0</v>
       </c>
       <c r="B20" t="n">
-        <v>35.0</v>
+        <v>53.0</v>
       </c>
       <c r="C20" t="n">
-        <v>50.0</v>
+        <v>44.0</v>
       </c>
       <c r="D20" t="n">
-        <v>50.0</v>
+        <v>39.0</v>
+      </c>
+      <c r="E20" t="n">
+        <v>49.0</v>
       </c>
     </row>
     <row r="21">
@@ -1522,13 +2378,16 @@
         <v>19.0</v>
       </c>
       <c r="B21" t="n">
-        <v>36.0</v>
+        <v>53.0</v>
       </c>
       <c r="C21" t="n">
-        <v>50.0</v>
+        <v>44.0</v>
       </c>
       <c r="D21" t="n">
-        <v>50.0</v>
+        <v>39.0</v>
+      </c>
+      <c r="E21" t="n">
+        <v>47.0</v>
       </c>
     </row>
     <row r="22">
@@ -1536,13 +2395,16 @@
         <v>20.0</v>
       </c>
       <c r="B22" t="n">
+        <v>53.0</v>
+      </c>
+      <c r="C22" t="n">
+        <v>43.0</v>
+      </c>
+      <c r="D22" t="n">
         <v>38.0</v>
       </c>
-      <c r="C22" t="n">
-        <v>50.0</v>
-      </c>
-      <c r="D22" t="n">
-        <v>50.0</v>
+      <c r="E22" t="n">
+        <v>46.0</v>
       </c>
     </row>
     <row r="23">
@@ -1550,13 +2412,16 @@
         <v>21.0</v>
       </c>
       <c r="B23" t="n">
-        <v>40.0</v>
+        <v>53.0</v>
       </c>
       <c r="C23" t="n">
-        <v>50.0</v>
+        <v>38.0</v>
       </c>
       <c r="D23" t="n">
-        <v>50.0</v>
+        <v>42.0</v>
+      </c>
+      <c r="E23" t="n">
+        <v>47.0</v>
       </c>
     </row>
     <row r="24">
@@ -1564,13 +2429,16 @@
         <v>22.0</v>
       </c>
       <c r="B24" t="n">
-        <v>40.0</v>
+        <v>53.0</v>
       </c>
       <c r="C24" t="n">
-        <v>50.0</v>
+        <v>38.0</v>
       </c>
       <c r="D24" t="n">
-        <v>50.0</v>
+        <v>47.0</v>
+      </c>
+      <c r="E24" t="n">
+        <v>41.0</v>
       </c>
     </row>
     <row r="25">
@@ -1578,13 +2446,16 @@
         <v>23.0</v>
       </c>
       <c r="B25" t="n">
-        <v>40.0</v>
+        <v>53.0</v>
       </c>
       <c r="C25" t="n">
-        <v>50.0</v>
+        <v>38.0</v>
       </c>
       <c r="D25" t="n">
-        <v>50.0</v>
+        <v>48.0</v>
+      </c>
+      <c r="E25" t="n">
+        <v>42.0</v>
       </c>
     </row>
     <row r="26">
@@ -1592,13 +2463,16 @@
         <v>24.0</v>
       </c>
       <c r="B26" t="n">
-        <v>41.0</v>
+        <v>53.0</v>
       </c>
       <c r="C26" t="n">
-        <v>50.0</v>
+        <v>38.0</v>
       </c>
       <c r="D26" t="n">
-        <v>50.0</v>
+        <v>48.0</v>
+      </c>
+      <c r="E26" t="n">
+        <v>42.0</v>
       </c>
     </row>
     <row r="27">
@@ -1606,13 +2480,16 @@
         <v>25.0</v>
       </c>
       <c r="B27" t="n">
-        <v>41.0</v>
+        <v>53.0</v>
       </c>
       <c r="C27" t="n">
-        <v>50.0</v>
+        <v>37.0</v>
       </c>
       <c r="D27" t="n">
-        <v>50.0</v>
+        <v>48.0</v>
+      </c>
+      <c r="E27" t="n">
+        <v>42.0</v>
       </c>
     </row>
     <row r="28">
@@ -1620,13 +2497,16 @@
         <v>26.0</v>
       </c>
       <c r="B28" t="n">
-        <v>40.0</v>
+        <v>53.0</v>
       </c>
       <c r="C28" t="n">
-        <v>50.0</v>
+        <v>37.0</v>
       </c>
       <c r="D28" t="n">
-        <v>50.0</v>
+        <v>49.0</v>
+      </c>
+      <c r="E28" t="n">
+        <v>43.0</v>
       </c>
     </row>
     <row r="29">
@@ -1634,13 +2514,16 @@
         <v>27.0</v>
       </c>
       <c r="B29" t="n">
-        <v>40.0</v>
+        <v>53.0</v>
       </c>
       <c r="C29" t="n">
         <v>50.0</v>
       </c>
       <c r="D29" t="n">
-        <v>50.0</v>
+        <v>44.0</v>
+      </c>
+      <c r="E29" t="n">
+        <v>37.0</v>
       </c>
     </row>
     <row r="30">
@@ -1648,13 +2531,16 @@
         <v>28.0</v>
       </c>
       <c r="B30" t="n">
-        <v>40.0</v>
+        <v>53.0</v>
       </c>
       <c r="C30" t="n">
-        <v>50.0</v>
+        <v>49.0</v>
       </c>
       <c r="D30" t="n">
-        <v>50.0</v>
+        <v>44.0</v>
+      </c>
+      <c r="E30" t="n">
+        <v>37.0</v>
       </c>
     </row>
     <row r="31">
@@ -1662,13 +2548,16 @@
         <v>29.0</v>
       </c>
       <c r="B31" t="n">
-        <v>40.0</v>
+        <v>55.0</v>
       </c>
       <c r="C31" t="n">
-        <v>50.0</v>
+        <v>44.0</v>
       </c>
       <c r="D31" t="n">
-        <v>50.0</v>
+        <v>37.0</v>
+      </c>
+      <c r="E31" t="n">
+        <v>48.0</v>
       </c>
     </row>
     <row r="32">
@@ -1676,13 +2565,16 @@
         <v>30.0</v>
       </c>
       <c r="B32" t="n">
-        <v>40.0</v>
+        <v>56.0</v>
       </c>
       <c r="C32" t="n">
-        <v>50.0</v>
+        <v>37.0</v>
       </c>
       <c r="D32" t="n">
-        <v>50.0</v>
+        <v>44.0</v>
+      </c>
+      <c r="E32" t="n">
+        <v>48.0</v>
       </c>
     </row>
     <row r="33">
@@ -1690,13 +2582,16 @@
         <v>31.0</v>
       </c>
       <c r="B33" t="n">
-        <v>39.0</v>
+        <v>56.0</v>
       </c>
       <c r="C33" t="n">
-        <v>50.0</v>
+        <v>44.0</v>
       </c>
       <c r="D33" t="n">
-        <v>50.0</v>
+        <v>37.0</v>
+      </c>
+      <c r="E33" t="n">
+        <v>48.0</v>
       </c>
     </row>
     <row r="34">
@@ -1704,13 +2599,16 @@
         <v>32.0</v>
       </c>
       <c r="B34" t="n">
-        <v>39.0</v>
+        <v>56.0</v>
       </c>
       <c r="C34" t="n">
-        <v>50.0</v>
+        <v>37.0</v>
       </c>
       <c r="D34" t="n">
-        <v>50.0</v>
+        <v>48.0</v>
+      </c>
+      <c r="E34" t="n">
+        <v>45.0</v>
       </c>
     </row>
     <row r="35">
@@ -1718,13 +2616,16 @@
         <v>33.0</v>
       </c>
       <c r="B35" t="n">
-        <v>38.0</v>
+        <v>56.0</v>
       </c>
       <c r="C35" t="n">
-        <v>50.0</v>
+        <v>36.0</v>
       </c>
       <c r="D35" t="n">
-        <v>50.0</v>
+        <v>49.0</v>
+      </c>
+      <c r="E35" t="n">
+        <v>45.0</v>
       </c>
     </row>
     <row r="36">
@@ -1732,13 +2633,16 @@
         <v>34.0</v>
       </c>
       <c r="B36" t="n">
-        <v>38.0</v>
+        <v>56.0</v>
       </c>
       <c r="C36" t="n">
-        <v>50.0</v>
+        <v>34.0</v>
       </c>
       <c r="D36" t="n">
-        <v>50.0</v>
+        <v>49.0</v>
+      </c>
+      <c r="E36" t="n">
+        <v>44.0</v>
       </c>
     </row>
     <row r="37">
@@ -1746,13 +2650,16 @@
         <v>35.0</v>
       </c>
       <c r="B37" t="n">
-        <v>38.0</v>
+        <v>56.0</v>
       </c>
       <c r="C37" t="n">
-        <v>50.0</v>
+        <v>32.0</v>
       </c>
       <c r="D37" t="n">
-        <v>50.0</v>
+        <v>49.0</v>
+      </c>
+      <c r="E37" t="n">
+        <v>43.0</v>
       </c>
     </row>
     <row r="38">
@@ -1760,13 +2667,16 @@
         <v>36.0</v>
       </c>
       <c r="B38" t="n">
-        <v>38.0</v>
+        <v>56.0</v>
       </c>
       <c r="C38" t="n">
-        <v>50.0</v>
+        <v>32.0</v>
       </c>
       <c r="D38" t="n">
-        <v>50.0</v>
+        <v>49.0</v>
+      </c>
+      <c r="E38" t="n">
+        <v>43.0</v>
       </c>
     </row>
     <row r="39">
@@ -1774,13 +2684,16 @@
         <v>37.0</v>
       </c>
       <c r="B39" t="n">
-        <v>38.0</v>
+        <v>56.0</v>
       </c>
       <c r="C39" t="n">
-        <v>50.0</v>
+        <v>32.0</v>
       </c>
       <c r="D39" t="n">
-        <v>50.0</v>
+        <v>49.0</v>
+      </c>
+      <c r="E39" t="n">
+        <v>44.0</v>
       </c>
     </row>
     <row r="40">
@@ -1788,13 +2701,16 @@
         <v>38.0</v>
       </c>
       <c r="B40" t="n">
-        <v>38.0</v>
+        <v>56.0</v>
       </c>
       <c r="C40" t="n">
-        <v>50.0</v>
+        <v>30.0</v>
       </c>
       <c r="D40" t="n">
-        <v>50.0</v>
+        <v>49.0</v>
+      </c>
+      <c r="E40" t="n">
+        <v>45.0</v>
       </c>
     </row>
     <row r="41">
@@ -1802,13 +2718,16 @@
         <v>39.0</v>
       </c>
       <c r="B41" t="n">
-        <v>39.0</v>
+        <v>56.0</v>
       </c>
       <c r="C41" t="n">
-        <v>50.0</v>
+        <v>48.0</v>
       </c>
       <c r="D41" t="n">
-        <v>50.0</v>
+        <v>30.0</v>
+      </c>
+      <c r="E41" t="n">
+        <v>45.0</v>
       </c>
     </row>
     <row r="42">
@@ -1816,13 +2735,16 @@
         <v>40.0</v>
       </c>
       <c r="B42" t="n">
-        <v>39.0</v>
+        <v>56.0</v>
       </c>
       <c r="C42" t="n">
-        <v>50.0</v>
+        <v>45.0</v>
       </c>
       <c r="D42" t="n">
-        <v>50.0</v>
+        <v>48.0</v>
+      </c>
+      <c r="E42" t="n">
+        <v>30.0</v>
       </c>
     </row>
     <row r="43">
@@ -1830,13 +2752,16 @@
         <v>41.0</v>
       </c>
       <c r="B43" t="n">
-        <v>39.0</v>
+        <v>56.0</v>
       </c>
       <c r="C43" t="n">
-        <v>50.0</v>
+        <v>49.0</v>
       </c>
       <c r="D43" t="n">
-        <v>50.0</v>
+        <v>45.0</v>
+      </c>
+      <c r="E43" t="n">
+        <v>29.0</v>
       </c>
     </row>
     <row r="44">
@@ -1844,13 +2769,16 @@
         <v>42.0</v>
       </c>
       <c r="B44" t="n">
-        <v>39.0</v>
+        <v>56.0</v>
       </c>
       <c r="C44" t="n">
-        <v>50.0</v>
+        <v>49.0</v>
       </c>
       <c r="D44" t="n">
-        <v>50.0</v>
+        <v>45.0</v>
+      </c>
+      <c r="E44" t="n">
+        <v>29.0</v>
       </c>
     </row>
     <row r="45">
@@ -1858,13 +2786,16 @@
         <v>43.0</v>
       </c>
       <c r="B45" t="n">
-        <v>40.0</v>
+        <v>56.0</v>
       </c>
       <c r="C45" t="n">
-        <v>50.0</v>
+        <v>49.0</v>
       </c>
       <c r="D45" t="n">
-        <v>50.0</v>
+        <v>45.0</v>
+      </c>
+      <c r="E45" t="n">
+        <v>29.0</v>
       </c>
     </row>
     <row r="46">
@@ -1872,13 +2803,16 @@
         <v>44.0</v>
       </c>
       <c r="B46" t="n">
-        <v>40.0</v>
+        <v>57.0</v>
       </c>
       <c r="C46" t="n">
-        <v>50.0</v>
+        <v>49.0</v>
       </c>
       <c r="D46" t="n">
-        <v>50.0</v>
+        <v>45.0</v>
+      </c>
+      <c r="E46" t="n">
+        <v>29.0</v>
       </c>
     </row>
     <row r="47">
@@ -1886,13 +2820,16 @@
         <v>45.0</v>
       </c>
       <c r="B47" t="n">
-        <v>40.0</v>
+        <v>58.0</v>
       </c>
       <c r="C47" t="n">
-        <v>50.0</v>
+        <v>45.0</v>
       </c>
       <c r="D47" t="n">
-        <v>50.0</v>
+        <v>48.0</v>
+      </c>
+      <c r="E47" t="n">
+        <v>29.0</v>
       </c>
     </row>
     <row r="48">
@@ -1900,13 +2837,16 @@
         <v>46.0</v>
       </c>
       <c r="B48" t="n">
-        <v>39.0</v>
+        <v>58.0</v>
       </c>
       <c r="C48" t="n">
-        <v>50.0</v>
+        <v>47.0</v>
       </c>
       <c r="D48" t="n">
-        <v>50.0</v>
+        <v>45.0</v>
+      </c>
+      <c r="E48" t="n">
+        <v>29.0</v>
       </c>
     </row>
     <row r="49">
@@ -1914,13 +2854,16 @@
         <v>47.0</v>
       </c>
       <c r="B49" t="n">
-        <v>38.0</v>
+        <v>59.0</v>
       </c>
       <c r="C49" t="n">
-        <v>50.0</v>
+        <v>45.0</v>
       </c>
       <c r="D49" t="n">
-        <v>50.0</v>
+        <v>47.0</v>
+      </c>
+      <c r="E49" t="n">
+        <v>29.0</v>
       </c>
     </row>
     <row r="50">
@@ -1928,13 +2871,16 @@
         <v>48.0</v>
       </c>
       <c r="B50" t="n">
-        <v>38.0</v>
+        <v>59.0</v>
       </c>
       <c r="C50" t="n">
-        <v>50.0</v>
+        <v>45.0</v>
       </c>
       <c r="D50" t="n">
-        <v>50.0</v>
+        <v>47.0</v>
+      </c>
+      <c r="E50" t="n">
+        <v>29.0</v>
       </c>
     </row>
     <row r="51">
@@ -1942,13 +2888,16 @@
         <v>49.0</v>
       </c>
       <c r="B51" t="n">
-        <v>36.0</v>
+        <v>59.0</v>
       </c>
       <c r="C51" t="n">
-        <v>50.0</v>
+        <v>45.0</v>
       </c>
       <c r="D51" t="n">
-        <v>50.0</v>
+        <v>46.0</v>
+      </c>
+      <c r="E51" t="n">
+        <v>29.0</v>
       </c>
     </row>
     <row r="52">
@@ -1956,13 +2905,16 @@
         <v>50.0</v>
       </c>
       <c r="B52" t="n">
-        <v>36.0</v>
+        <v>59.0</v>
       </c>
       <c r="C52" t="n">
-        <v>50.0</v>
+        <v>45.0</v>
       </c>
       <c r="D52" t="n">
-        <v>50.0</v>
+        <v>46.0</v>
+      </c>
+      <c r="E52" t="n">
+        <v>28.0</v>
       </c>
     </row>
     <row r="53">
@@ -1970,13 +2922,16 @@
         <v>51.0</v>
       </c>
       <c r="B53" t="n">
-        <v>37.0</v>
+        <v>59.0</v>
       </c>
       <c r="C53" t="n">
-        <v>50.0</v>
+        <v>44.0</v>
       </c>
       <c r="D53" t="n">
-        <v>50.0</v>
+        <v>45.0</v>
+      </c>
+      <c r="E53" t="n">
+        <v>28.0</v>
       </c>
     </row>
     <row r="54">
@@ -1984,13 +2939,16 @@
         <v>52.0</v>
       </c>
       <c r="B54" t="n">
-        <v>37.0</v>
+        <v>60.0</v>
       </c>
       <c r="C54" t="n">
-        <v>50.0</v>
+        <v>43.0</v>
       </c>
       <c r="D54" t="n">
-        <v>50.0</v>
+        <v>46.0</v>
+      </c>
+      <c r="E54" t="n">
+        <v>28.0</v>
       </c>
     </row>
     <row r="55">
@@ -1998,13 +2956,16 @@
         <v>53.0</v>
       </c>
       <c r="B55" t="n">
-        <v>36.0</v>
+        <v>61.0</v>
       </c>
       <c r="C55" t="n">
-        <v>50.0</v>
+        <v>43.0</v>
       </c>
       <c r="D55" t="n">
-        <v>50.0</v>
+        <v>47.0</v>
+      </c>
+      <c r="E55" t="n">
+        <v>26.0</v>
       </c>
     </row>
     <row r="56">
@@ -2012,13 +2973,16 @@
         <v>54.0</v>
       </c>
       <c r="B56" t="n">
-        <v>36.0</v>
+        <v>61.0</v>
       </c>
       <c r="C56" t="n">
-        <v>50.0</v>
+        <v>43.0</v>
       </c>
       <c r="D56" t="n">
-        <v>50.0</v>
+        <v>47.0</v>
+      </c>
+      <c r="E56" t="n">
+        <v>26.0</v>
       </c>
     </row>
     <row r="57">
@@ -2026,13 +2990,16 @@
         <v>55.0</v>
       </c>
       <c r="B57" t="n">
-        <v>37.0</v>
+        <v>61.0</v>
       </c>
       <c r="C57" t="n">
-        <v>50.0</v>
+        <v>41.0</v>
       </c>
       <c r="D57" t="n">
-        <v>50.0</v>
+        <v>47.0</v>
+      </c>
+      <c r="E57" t="n">
+        <v>26.0</v>
       </c>
     </row>
     <row r="58">
@@ -2040,13 +3007,16 @@
         <v>56.0</v>
       </c>
       <c r="B58" t="n">
-        <v>37.0</v>
+        <v>61.0</v>
       </c>
       <c r="C58" t="n">
-        <v>50.0</v>
+        <v>41.0</v>
       </c>
       <c r="D58" t="n">
-        <v>50.0</v>
+        <v>47.0</v>
+      </c>
+      <c r="E58" t="n">
+        <v>25.0</v>
       </c>
     </row>
     <row r="59">
@@ -2054,13 +3024,16 @@
         <v>57.0</v>
       </c>
       <c r="B59" t="n">
-        <v>37.0</v>
+        <v>61.0</v>
       </c>
       <c r="C59" t="n">
-        <v>50.0</v>
+        <v>47.0</v>
       </c>
       <c r="D59" t="n">
-        <v>50.0</v>
+        <v>41.0</v>
+      </c>
+      <c r="E59" t="n">
+        <v>25.0</v>
       </c>
     </row>
     <row r="60">
@@ -2068,13 +3041,16 @@
         <v>58.0</v>
       </c>
       <c r="B60" t="n">
-        <v>37.0</v>
+        <v>61.0</v>
       </c>
       <c r="C60" t="n">
-        <v>50.0</v>
+        <v>47.0</v>
       </c>
       <c r="D60" t="n">
-        <v>50.0</v>
+        <v>41.0</v>
+      </c>
+      <c r="E60" t="n">
+        <v>25.0</v>
       </c>
     </row>
     <row r="61">
@@ -2082,13 +3058,16 @@
         <v>59.0</v>
       </c>
       <c r="B61" t="n">
-        <v>38.0</v>
+        <v>61.0</v>
       </c>
       <c r="C61" t="n">
-        <v>50.0</v>
+        <v>41.0</v>
       </c>
       <c r="D61" t="n">
-        <v>50.0</v>
+        <v>46.0</v>
+      </c>
+      <c r="E61" t="n">
+        <v>25.0</v>
       </c>
     </row>
     <row r="62">
@@ -2096,13 +3075,16 @@
         <v>60.0</v>
       </c>
       <c r="B62" t="n">
-        <v>37.0</v>
+        <v>61.0</v>
       </c>
       <c r="C62" t="n">
-        <v>50.0</v>
+        <v>41.0</v>
       </c>
       <c r="D62" t="n">
-        <v>50.0</v>
+        <v>47.0</v>
+      </c>
+      <c r="E62" t="n">
+        <v>25.0</v>
       </c>
     </row>
     <row r="63">
@@ -2110,13 +3092,16 @@
         <v>61.0</v>
       </c>
       <c r="B63" t="n">
-        <v>36.0</v>
+        <v>61.0</v>
       </c>
       <c r="C63" t="n">
-        <v>50.0</v>
+        <v>42.0</v>
       </c>
       <c r="D63" t="n">
-        <v>50.0</v>
+        <v>47.0</v>
+      </c>
+      <c r="E63" t="n">
+        <v>25.0</v>
       </c>
     </row>
     <row r="64">
@@ -2124,13 +3109,16 @@
         <v>62.0</v>
       </c>
       <c r="B64" t="n">
-        <v>36.0</v>
+        <v>62.0</v>
       </c>
       <c r="C64" t="n">
-        <v>50.0</v>
+        <v>41.0</v>
       </c>
       <c r="D64" t="n">
-        <v>50.0</v>
+        <v>47.0</v>
+      </c>
+      <c r="E64" t="n">
+        <v>25.0</v>
       </c>
     </row>
     <row r="65">
@@ -2138,13 +3126,16 @@
         <v>63.0</v>
       </c>
       <c r="B65" t="n">
-        <v>37.0</v>
+        <v>62.0</v>
       </c>
       <c r="C65" t="n">
-        <v>50.0</v>
+        <v>41.0</v>
       </c>
       <c r="D65" t="n">
-        <v>50.0</v>
+        <v>46.0</v>
+      </c>
+      <c r="E65" t="n">
+        <v>25.0</v>
       </c>
     </row>
     <row r="66">
@@ -2152,13 +3143,16 @@
         <v>64.0</v>
       </c>
       <c r="B66" t="n">
-        <v>36.0</v>
+        <v>62.0</v>
       </c>
       <c r="C66" t="n">
-        <v>50.0</v>
+        <v>41.0</v>
       </c>
       <c r="D66" t="n">
-        <v>50.0</v>
+        <v>45.0</v>
+      </c>
+      <c r="E66" t="n">
+        <v>25.0</v>
       </c>
     </row>
     <row r="67">
@@ -2166,13 +3160,16 @@
         <v>65.0</v>
       </c>
       <c r="B67" t="n">
-        <v>36.0</v>
+        <v>62.0</v>
       </c>
       <c r="C67" t="n">
-        <v>50.0</v>
+        <v>40.0</v>
       </c>
       <c r="D67" t="n">
-        <v>50.0</v>
+        <v>47.0</v>
+      </c>
+      <c r="E67" t="n">
+        <v>25.0</v>
       </c>
     </row>
     <row r="68">
@@ -2180,13 +3177,16 @@
         <v>66.0</v>
       </c>
       <c r="B68" t="n">
-        <v>36.0</v>
+        <v>63.0</v>
       </c>
       <c r="C68" t="n">
-        <v>50.0</v>
+        <v>40.0</v>
       </c>
       <c r="D68" t="n">
-        <v>50.0</v>
+        <v>48.0</v>
+      </c>
+      <c r="E68" t="n">
+        <v>25.0</v>
       </c>
     </row>
     <row r="69">
@@ -2194,13 +3194,16 @@
         <v>67.0</v>
       </c>
       <c r="B69" t="n">
-        <v>36.0</v>
+        <v>63.0</v>
       </c>
       <c r="C69" t="n">
-        <v>50.0</v>
+        <v>40.0</v>
       </c>
       <c r="D69" t="n">
-        <v>50.0</v>
+        <v>49.0</v>
+      </c>
+      <c r="E69" t="n">
+        <v>24.0</v>
       </c>
     </row>
     <row r="70">
@@ -2208,13 +3211,16 @@
         <v>68.0</v>
       </c>
       <c r="B70" t="n">
-        <v>36.0</v>
+        <v>63.0</v>
       </c>
       <c r="C70" t="n">
-        <v>50.0</v>
+        <v>40.0</v>
       </c>
       <c r="D70" t="n">
         <v>50.0</v>
+      </c>
+      <c r="E70" t="n">
+        <v>23.0</v>
       </c>
     </row>
     <row r="71">
@@ -2222,13 +3228,16 @@
         <v>69.0</v>
       </c>
       <c r="B71" t="n">
-        <v>37.0</v>
+        <v>63.0</v>
       </c>
       <c r="C71" t="n">
-        <v>50.0</v>
+        <v>40.0</v>
       </c>
       <c r="D71" t="n">
         <v>50.0</v>
+      </c>
+      <c r="E71" t="n">
+        <v>23.0</v>
       </c>
     </row>
     <row r="72">
@@ -2236,153 +3245,16 @@
         <v>70.0</v>
       </c>
       <c r="B72" t="n">
-        <v>37.0</v>
+        <v>63.0</v>
       </c>
       <c r="C72" t="n">
-        <v>50.0</v>
+        <v>39.0</v>
       </c>
       <c r="D72" t="n">
-        <v>50.0</v>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" t="n">
-        <v>71.0</v>
-      </c>
-      <c r="B73" t="n">
-        <v>37.0</v>
-      </c>
-      <c r="C73" t="n">
-        <v>50.0</v>
-      </c>
-      <c r="D73" t="n">
-        <v>50.0</v>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" t="n">
-        <v>72.0</v>
-      </c>
-      <c r="B74" t="n">
-        <v>38.0</v>
-      </c>
-      <c r="C74" t="n">
-        <v>50.0</v>
-      </c>
-      <c r="D74" t="n">
-        <v>50.0</v>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" t="n">
-        <v>73.0</v>
-      </c>
-      <c r="B75" t="n">
-        <v>37.0</v>
-      </c>
-      <c r="C75" t="n">
-        <v>50.0</v>
-      </c>
-      <c r="D75" t="n">
-        <v>50.0</v>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" t="n">
-        <v>74.0</v>
-      </c>
-      <c r="B76" t="n">
-        <v>37.0</v>
-      </c>
-      <c r="C76" t="n">
-        <v>50.0</v>
-      </c>
-      <c r="D76" t="n">
-        <v>50.0</v>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" t="n">
-        <v>75.0</v>
-      </c>
-      <c r="B77" t="n">
-        <v>37.0</v>
-      </c>
-      <c r="C77" t="n">
-        <v>50.0</v>
-      </c>
-      <c r="D77" t="n">
-        <v>50.0</v>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" t="n">
-        <v>76.0</v>
-      </c>
-      <c r="B78" t="n">
-        <v>38.0</v>
-      </c>
-      <c r="C78" t="n">
-        <v>50.0</v>
-      </c>
-      <c r="D78" t="n">
-        <v>50.0</v>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" t="n">
-        <v>77.0</v>
-      </c>
-      <c r="B79" t="n">
-        <v>40.0</v>
-      </c>
-      <c r="C79" t="n">
-        <v>50.0</v>
-      </c>
-      <c r="D79" t="n">
-        <v>50.0</v>
-      </c>
-    </row>
-    <row r="80">
-      <c r="A80" t="n">
-        <v>78.0</v>
-      </c>
-      <c r="B80" t="n">
-        <v>40.0</v>
-      </c>
-      <c r="C80" t="n">
-        <v>50.0</v>
-      </c>
-      <c r="D80" t="n">
-        <v>50.0</v>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" t="n">
-        <v>79.0</v>
-      </c>
-      <c r="B81" t="n">
-        <v>40.0</v>
-      </c>
-      <c r="C81" t="n">
-        <v>50.0</v>
-      </c>
-      <c r="D81" t="n">
-        <v>50.0</v>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" t="n">
-        <v>80.0</v>
-      </c>
-      <c r="B82" t="n">
-        <v>41.0</v>
-      </c>
-      <c r="C82" t="n">
-        <v>50.0</v>
-      </c>
-      <c r="D82" t="n">
-        <v>50.0</v>
+        <v>49.0</v>
+      </c>
+      <c r="E72" t="n">
+        <v>23.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>